<commit_message>
updated old template samples
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
+++ b/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="no" vbProcedure="false">Sheet1!$M$37</definedName>
+    <definedName function="false" hidden="false" name="no" vbProcedure="false">Sheet1!$N$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,14 +23,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="171">
   <si>
     <t xml:space="preserve">SOFTWARE QUALITY GRADE</t>
   </si>
   <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Summary Information (All)</t>
   </si>
   <si>
+    <t xml:space="preserve">WORKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS BUT MANUALLY INSTALL ALL TOOLS; OF THE PROVIDED SCRIPT USE tools/install.sh rdep for dependencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUST HAVE GPU WITH CUDA (https://groups.google.com/forum/?fromgroups#!topic/sailfish-cfd/jpeuBeO8k2k), also installed pyopencl first as had issues last, add scikit-image, and python path, run using python2.7 – instructions are in several spots (not linear); posted on their discussion board but unclear if checked, if no answer may try http://mjanusz.github.io/homepage/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNCLEAR IF WORKING CORRECTLY, SENT EMAIL; ran make in lower LUMA, copied makefile up 1 dir, need install paraview but output seems off (asked about this), test cases are not clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNW SENT EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received response -works well now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEAD &amp; no clear contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEAD – UNCLEAR HOW TO IMPLEMENT, AND DID NOT RESPOND TO CONTACT FROM OTHER USER ISSUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Software Name:</t>
   </si>
   <si>
@@ -44,6 +71,24 @@
   </si>
   <si>
     <t xml:space="preserve">LUMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HemeLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laboetie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBSim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lettuce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loliverhennigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palabos</t>
   </si>
   <si>
     <t xml:space="preserve">URL:</t>
@@ -502,7 +547,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]MMM\-YY"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -554,12 +599,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="13.5"/>
@@ -646,7 +685,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -679,6 +718,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -687,11 +730,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -703,11 +746,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,7 +762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,11 +770,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -817,45 +860,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE451"/>
+  <dimension ref="A1:AF131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D132" activeCellId="0" sqref="D132"/>
+      <selection pane="bottomLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.96875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="17.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="20.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,138 +909,202 @@
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
+      <c r="I2" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>1</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y7" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>73</v>
@@ -1011,47 +1118,47 @@
       <c r="E8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="AE8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="AF8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2007</v>
@@ -1065,15 +1172,15 @@
       <c r="E11" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>2020</v>
@@ -1087,189 +1194,189 @@
       <c r="E12" s="0" t="n">
         <v>2020</v>
       </c>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD14" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="AE14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>46</v>
+        <v>59</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>49</v>
+        <v>63</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,12 +1384,12 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1397,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,86 +1405,86 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z28" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="AA28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>5</v>
@@ -1394,7 +1501,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>11</v>
@@ -1410,25 +1517,25 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
-        <v>70</v>
+      <c r="A36" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
-        <v>72</v>
+      <c r="A37" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>4</v>
@@ -1444,84 +1551,84 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
-        <v>75</v>
+      <c r="A41" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
-        <v>76</v>
+      <c r="A42" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
-        <v>72</v>
+      <c r="A44" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>4</v>
@@ -1535,55 +1642,55 @@
       <c r="E44" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Z44" s="16"/>
+      <c r="AA44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="17" t="n">
+      <c r="A49" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="18" t="n">
         <v>4</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -1601,49 +1708,49 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N52" s="15"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="M52" s="14"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="17" t="n">
+      <c r="B54" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="0" t="n">
@@ -1661,157 +1768,157 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="17"/>
+      <c r="A58" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="18"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
-        <v>99</v>
+      <c r="A68" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="17" t="n">
+      <c r="A69" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="18" t="n">
         <v>7</v>
       </c>
       <c r="C69" s="0" t="n">
@@ -1825,171 +1932,171 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="14"/>
+      <c r="A70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="17" t="n">
+      <c r="A81" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" s="18" t="n">
         <v>8</v>
       </c>
       <c r="C81" s="0" t="n">
@@ -2007,48 +2114,48 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" s="17" t="n">
+      <c r="A86" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C86" s="0" t="n">
@@ -2066,83 +2173,83 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="14" t="s">
-        <v>119</v>
+      <c r="A89" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F89" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="G89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="14" t="s">
-        <v>121</v>
+      <c r="A90" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="14" t="s">
-        <v>123</v>
+      <c r="A92" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B93" s="17" t="n">
+      <c r="A93" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C93" s="0" t="n">
@@ -2160,189 +2267,189 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="14" t="s">
-        <v>126</v>
+      <c r="A97" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="14" t="s">
-        <v>127</v>
+      <c r="A98" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="14" t="s">
-        <v>128</v>
+      <c r="A99" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="14" t="s">
-        <v>129</v>
+      <c r="A100" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="14" t="s">
-        <v>130</v>
+      <c r="A101" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="14" t="s">
-        <v>131</v>
+      <c r="A102" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B105" s="19" t="s">
-        <v>51</v>
+      <c r="A105" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>78</v>
+        <v>150</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B107" s="17" t="n">
+      <c r="A107" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107" s="18" t="n">
         <v>6</v>
       </c>
       <c r="C107" s="0" t="n">
@@ -2357,71 +2464,71 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="6"/>
-      <c r="B108" s="20"/>
+      <c r="B108" s="21"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q110" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="R110" s="10"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="14" t="s">
-        <v>140</v>
+      <c r="A112" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N112" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="O112" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B113" s="17" t="n">
+      <c r="A113" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C113" s="0" t="n">
@@ -2439,29 +2546,29 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="14" t="s">
-        <v>142</v>
+      <c r="A116" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="6" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B117" s="1" t="n">
         <v>5</v>
@@ -2477,10 +2584,10 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B118" s="17" t="n">
+      <c r="A118" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B118" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C118" s="0" t="n">
@@ -2498,65 +2605,65 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="6" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="21" t="s">
-        <v>146</v>
+      <c r="A122" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="14" t="s">
-        <v>147</v>
+      <c r="A123" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B124" s="17" t="n">
+      <c r="A124" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B124" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C124" s="0" t="n">
@@ -2574,42 +2681,42 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q126" s="9"/>
+        <v>163</v>
+      </c>
+      <c r="R126" s="10"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="6" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="6" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,332 +2724,12 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K131" s="22"/>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L131" s="23"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated comments on LUMA and Sailfish from dev responses
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
+++ b/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">MUST HAVE GPU WITH CUDA (https://groups.google.com/forum/?fromgroups#!topic/sailfish-cfd/jpeuBeO8k2k), also installed pyopencl first as had issues last, add scikit-image, and python path, run using python2.7 – instructions are in several spots (not linear); posted on their discussion board but unclear if checked, if no answer may try http://mjanusz.github.io/homepage/</t>
   </si>
   <si>
-    <t xml:space="preserve">UNCLEAR IF WORKING CORRECTLY, SENT EMAIL; ran make in lower LUMA, copied makefile up 1 dir, need install paraview but output seems off (asked about this), test cases are not clear</t>
+    <t xml:space="preserve">UNCLEAR IF WORKING CORRECTLY, SENT EMAIL – RESPONSE DID NOT SOLVE NPROCS ISSUE (I DEFAULTED VALUES TO 1 TO MAKE THE CODE “WORK”, ADDITIONALLY THE RESPONSE INFORMED ME THAT ADDITIONAL LABOUR INTENSIVE PROGRAMMING IN VISUAL STUDIO IS NEEDED TO BUILD A SEPARATE TOOL IN ORDER TO HAVE VISUALIZED OUTPUT ON PARAVIEW, WITHOUT THIS ONLY  H5 FORMAT FOR FLUID PARAMETERS AVAILABLE; my notes: ran make in lower LUMA, copied makefile up 1 dir, need install paraview but output seems off (asked about this), test cases are not clear</t>
   </si>
   <si>
     <t xml:space="preserve">DNW SENT EMAIL</t>
@@ -865,7 +865,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updated time spent on installing/evaluating solvers
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
+++ b/StateOfPractice/Peter-Notes/OldTemplate_LatticeBoltzmannSolvers.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="175">
   <si>
     <t xml:space="preserve">SOFTWARE QUALITY GRADE</t>
   </si>
@@ -529,10 +529,22 @@
     <t xml:space="preserve">Time Required for assessment:</t>
   </si>
   <si>
-    <t xml:space="preserve">4hours</t>
+    <t xml:space="preserve">5hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2hrs</t>
   </si>
   <si>
     <t xml:space="preserve">3hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr</t>
   </si>
   <si>
     <t xml:space="preserve">AHP pair wise comparisons done separately</t>
@@ -863,14 +875,14 @@
   <dimension ref="A1:AF131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
@@ -2713,18 +2725,36 @@
         <v>169</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E128" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="G128" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="H128" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="J128" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="K128" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="L128" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="M128" s="0" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="6"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>